<commit_message>
generating labels from excel
</commit_message>
<xml_diff>
--- a/label.xlsx
+++ b/label.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0d34a9ad5701c86e/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/goose/GitHub/label_maker_tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{12B7386B-2B5F-A94F-A669-49167F5478A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A8B3A05-E8DB-6241-8E8A-22F8ECEEB98A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63560F26-2EE1-BB42-A612-D2B068F9847A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="500" windowWidth="28040" windowHeight="19520" xr2:uid="{E5D8437A-4CF3-624E-825B-073214BFC1C9}"/>
+    <workbookView xWindow="64840" yWindow="3740" windowWidth="28040" windowHeight="19520" xr2:uid="{E5D8437A-4CF3-624E-825B-073214BFC1C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>12q ED 01 a1</t>
-  </si>
-  <si>
     <t>333 ED 02 A2</t>
   </si>
   <si>
@@ -57,6 +54,9 @@
   </si>
   <si>
     <t>456 aa 01 a2</t>
+  </si>
+  <si>
+    <t>1dq ED 01 a1</t>
   </si>
 </sst>
 </file>
@@ -115,10 +115,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -421,7 +417,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -431,37 +427,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
read only column A
</commit_message>
<xml_diff>
--- a/label.xlsx
+++ b/label.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/goose/GitHub/label_maker_tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63560F26-2EE1-BB42-A612-D2B068F9847A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967EC013-A40E-464C-BEEC-4407D593887E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="64840" yWindow="3740" windowWidth="28040" windowHeight="19520" xr2:uid="{E5D8437A-4CF3-624E-825B-073214BFC1C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>333 ED 02 A2</t>
   </si>
@@ -414,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D25E5E8-D4DF-C04A-8CBB-42952B1F392D}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -425,38 +425,59 @@
     <col min="1" max="1" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated how to use
</commit_message>
<xml_diff>
--- a/label.xlsx
+++ b/label.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0d34a9ad5701c86e/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/goose/GitHub/label_maker_tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{12B7386B-2B5F-A94F-A669-49167F5478A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A8B3A05-E8DB-6241-8E8A-22F8ECEEB98A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CAA6F0F-CEC5-EF42-B7E4-EED57709E48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6060" yWindow="500" windowWidth="28040" windowHeight="19520" xr2:uid="{E5D8437A-4CF3-624E-825B-073214BFC1C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>12q ED 01 a1</t>
   </si>
@@ -44,9 +44,6 @@
     <t>333 ED 02 A2</t>
   </si>
   <si>
-    <t>label</t>
-  </si>
-  <si>
     <t>12q ED 01 a2</t>
   </si>
   <si>
@@ -57,6 +54,27 @@
   </si>
   <si>
     <t>456 aa 01 a2</t>
+  </si>
+  <si>
+    <t>www dd 33 b1</t>
+  </si>
+  <si>
+    <t>stp dd 33b2</t>
+  </si>
+  <si>
+    <t>444ED02A1</t>
+  </si>
+  <si>
+    <t>g2q,ED,01,a1</t>
+  </si>
+  <si>
+    <t>todo</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>502 ED 01 a2</t>
   </si>
 </sst>
 </file>
@@ -115,10 +133,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -418,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D25E5E8-D4DF-C04A-8CBB-42952B1F392D}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -429,39 +443,90 @@
     <col min="1" max="1" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>